<commit_message>
feat get probabilities + create tensor flow numpy
</commit_message>
<xml_diff>
--- a/sb_gbi/test_data_10.05.23.xlsx
+++ b/sb_gbi/test_data_10.05.23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matsz\programowanie\Optymalizacja portfela\sb_gbi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DB98EF-EAC3-4CAB-B779-9C4A3445E91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752AB85D-A6C1-47CD-BEB7-F4575EC8E2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{90D27AAA-C75B-4672-92D9-37A52F75E2C9}"/>
   </bookViews>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B858B7-6452-43F1-BC68-609EA63B3AB1}">
   <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1953,10 +1953,10 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="G37" s="3">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="H37" s="3">
         <v>10000</v>
@@ -1970,39 +1970,39 @@
       </c>
       <c r="K37">
         <f>J37*F37-D37</f>
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="L37">
         <f>J37*G37-E37</f>
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="M37" s="3">
         <f t="shared" ref="M37:M41" si="26">ROUNDDOWN(K37/B37,0)</f>
-        <v>200</v>
+        <v>266</v>
       </c>
       <c r="N37" s="3">
         <f t="shared" ref="N37:N41" si="27">ROUNDDOWN(L37/C37,0)</f>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="O37" s="3">
         <f>M37</f>
-        <v>200</v>
+        <v>266</v>
       </c>
       <c r="P37" s="3">
         <f>N37</f>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="Q37" s="3">
         <f>O37*B37+P37*C37</f>
-        <v>10000</v>
+        <v>9980</v>
       </c>
       <c r="R37" s="3">
         <f>Q37-J37</f>
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="S37">
         <f>M37*B37+N37*C37</f>
-        <v>10000</v>
+        <v>9980</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
@@ -2017,63 +2017,63 @@
       </c>
       <c r="D38">
         <f>O37*B38</f>
-        <v>6540.0000000000009</v>
+        <v>8698.2000000000007</v>
       </c>
       <c r="E38">
         <f>P37*C38</f>
-        <v>4120</v>
+        <v>2060</v>
       </c>
       <c r="F38">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="G38" s="3">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="H38" s="3">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="I38">
         <v>0</v>
       </c>
       <c r="J38" s="3">
         <f>D38+E38+H38-I38</f>
-        <v>10660</v>
+        <v>11758.2</v>
       </c>
       <c r="K38">
         <f>J38*F38-D38</f>
-        <v>-144.00000000000091</v>
+        <v>708.36000000000058</v>
       </c>
       <c r="L38">
         <f>J38*G38-E38</f>
-        <v>144</v>
+        <v>291.64000000000033</v>
       </c>
       <c r="M38" s="3">
         <f t="shared" si="26"/>
-        <v>-4</v>
+        <v>21</v>
       </c>
       <c r="N38" s="3">
         <f t="shared" si="27"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O38" s="3">
         <f>O37+M38</f>
-        <v>196</v>
+        <v>287</v>
       </c>
       <c r="P38" s="3">
         <f>P37+N38</f>
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="Q38" s="3">
         <f>O38*B38+P38*C38</f>
-        <v>10632.2</v>
+        <v>11702.400000000001</v>
       </c>
       <c r="R38" s="3">
         <f>Q38-J38</f>
-        <v>-27.799999999999272</v>
+        <v>-55.799999999999272</v>
       </c>
       <c r="S38">
         <f t="shared" ref="S38:S42" si="28">M38*B38+N38*C38</f>
-        <v>-27.800000000000011</v>
+        <v>944.2</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
@@ -2088,17 +2088,17 @@
       </c>
       <c r="D39">
         <f t="shared" ref="D39:D42" si="29">O38*B39</f>
-        <v>4935.28</v>
+        <v>7226.66</v>
       </c>
       <c r="E39">
         <f t="shared" ref="E39:E42" si="30">P38*C39</f>
-        <v>4603.4800000000005</v>
+        <v>2526.3000000000002</v>
       </c>
       <c r="F39">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="G39" s="3">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="H39" s="3">
         <v>1000</v>
@@ -2107,20 +2107,20 @@
         <v>0</v>
       </c>
       <c r="J39" s="3">
-        <f t="shared" ref="J39:J42" si="31">D39+E39+H39-I39</f>
-        <v>10538.76</v>
+        <f t="shared" ref="J39:J40" si="31">D39+E39+H39-I39</f>
+        <v>10752.96</v>
       </c>
       <c r="K39">
         <f t="shared" ref="K39:K42" si="32">J39*F39-D39</f>
-        <v>1387.9760000000006</v>
+        <v>1375.7080000000005</v>
       </c>
       <c r="L39">
         <f t="shared" ref="L39:L42" si="33">J39*G39-E39</f>
-        <v>-387.97600000000057</v>
+        <v>-375.70800000000008</v>
       </c>
       <c r="M39" s="3">
         <f t="shared" si="26"/>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N39" s="3">
         <f t="shared" si="27"/>
@@ -2128,23 +2128,23 @@
       </c>
       <c r="O39" s="3">
         <f t="shared" ref="O39:O42" si="34">O38+M39</f>
-        <v>251</v>
+        <v>341</v>
       </c>
       <c r="P39" s="3">
         <f t="shared" ref="P39:P42" si="35">P38+N39</f>
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="Q39" s="3">
         <f>O39*B39+P39*C39</f>
-        <v>10586.82</v>
+        <v>10775.84</v>
       </c>
       <c r="R39" s="3">
         <f>Q39-J39</f>
-        <v>48.059999999999491</v>
+        <v>22.880000000001019</v>
       </c>
       <c r="S39">
         <f t="shared" si="28"/>
-        <v>1048.06</v>
+        <v>1022.88</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
@@ -2159,11 +2159,11 @@
       </c>
       <c r="D40">
         <f t="shared" si="29"/>
-        <v>5941.17</v>
+        <v>8071.47</v>
       </c>
       <c r="E40">
         <f t="shared" si="30"/>
-        <v>4309.2</v>
+        <v>2211.3000000000002</v>
       </c>
       <c r="F40">
         <v>0.7</v>
@@ -2179,43 +2179,43 @@
       </c>
       <c r="J40" s="3">
         <f t="shared" si="31"/>
-        <v>11250.369999999999</v>
+        <v>11282.77</v>
       </c>
       <c r="K40">
         <f>J40*F40-D40</f>
-        <v>1934.088999999999</v>
+        <v>-173.53100000000086</v>
       </c>
       <c r="L40">
         <f t="shared" si="33"/>
-        <v>-934.0890000000004</v>
+        <v>1173.5309999999999</v>
       </c>
       <c r="M40" s="3">
         <f t="shared" si="26"/>
-        <v>81</v>
+        <v>-7</v>
       </c>
       <c r="N40" s="3">
         <f t="shared" si="27"/>
-        <v>-16</v>
+        <v>20</v>
       </c>
       <c r="O40" s="3">
         <f t="shared" si="34"/>
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="P40" s="3">
         <f t="shared" si="35"/>
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q40" s="3">
         <f>O40*B40+P40*C40</f>
-        <v>11260.44</v>
+        <v>11251.080000000002</v>
       </c>
       <c r="R40" s="3">
         <f>Q40-J40</f>
-        <v>10.070000000001528</v>
+        <v>-31.68999999999869</v>
       </c>
       <c r="S40">
         <f t="shared" si="28"/>
-        <v>1010.0700000000002</v>
+        <v>968.31</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
@@ -2230,11 +2230,11 @@
       </c>
       <c r="D41">
         <f t="shared" si="29"/>
-        <v>10135.960000000001</v>
+        <v>10197.02</v>
       </c>
       <c r="E41">
         <f t="shared" si="30"/>
-        <v>3469.7999999999997</v>
+        <v>3411.97</v>
       </c>
       <c r="F41">
         <v>0.6</v>
@@ -2249,24 +2249,24 @@
         <v>0</v>
       </c>
       <c r="J41" s="3">
-        <f t="shared" si="31"/>
-        <v>14605.76</v>
+        <f>D41+E41+H41-I41</f>
+        <v>14608.99</v>
       </c>
       <c r="K41">
         <f t="shared" si="32"/>
-        <v>-1372.5040000000008</v>
+        <v>-1431.6260000000002</v>
       </c>
       <c r="L41">
         <f t="shared" si="33"/>
-        <v>2372.5040000000004</v>
+        <v>2431.6260000000007</v>
       </c>
       <c r="M41" s="3">
         <f t="shared" si="26"/>
-        <v>-44</v>
+        <v>-46</v>
       </c>
       <c r="N41" s="3">
         <f t="shared" si="27"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O41" s="3">
         <f t="shared" si="34"/>
@@ -2282,11 +2282,11 @@
       </c>
       <c r="R41" s="3">
         <f>Q41-J41</f>
-        <v>27.709999999999127</v>
+        <v>24.479999999999563</v>
       </c>
       <c r="S41">
         <f t="shared" si="28"/>
-        <v>1027.7099999999996</v>
+        <v>1024.48</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.3">
@@ -2308,56 +2308,56 @@
         <v>6016.57</v>
       </c>
       <c r="F42">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="G42" s="3">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H42" s="3">
         <v>0</v>
       </c>
       <c r="I42" s="3">
-        <v>12692.936000000002</v>
+        <v>15000</v>
       </c>
       <c r="J42" s="3">
-        <f t="shared" si="31"/>
-        <v>3173.2339999999986</v>
+        <f>D42+E42+H42-I42</f>
+        <v>866.17000000000007</v>
       </c>
       <c r="K42">
         <f t="shared" si="32"/>
-        <v>-7945.6596000000009</v>
+        <v>-9416.5149999999994</v>
       </c>
       <c r="L42">
         <f t="shared" si="33"/>
-        <v>-4747.2764000000006</v>
+        <v>-5583.4849999999997</v>
       </c>
       <c r="M42" s="3">
         <f>ROUNDDOWN(K42/B42,0)</f>
-        <v>-232</v>
+        <v>-275</v>
       </c>
       <c r="N42" s="3">
         <f>ROUNDDOWN(L42/C42,0)</f>
-        <v>-79</v>
+        <v>-93</v>
       </c>
       <c r="O42" s="3">
         <f t="shared" si="34"/>
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="P42" s="3">
         <f t="shared" si="35"/>
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="Q42" s="3">
         <f>O42*B42+P42*C42</f>
-        <v>3225.7400000000002</v>
+        <v>921.16000000000008</v>
       </c>
       <c r="R42" s="3">
         <f>Q42-J42</f>
-        <v>52.506000000001677</v>
+        <v>54.990000000000009</v>
       </c>
       <c r="S42" s="3">
         <f t="shared" si="28"/>
-        <v>-12640.43</v>
+        <v>-14945.01</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
@@ -2377,15 +2377,15 @@
     <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="I44">
         <f>J42*0.8</f>
-        <v>2538.587199999999</v>
+        <v>692.93600000000015</v>
       </c>
       <c r="J44" s="3">
         <f>J42*F42</f>
-        <v>1903.940399999999</v>
+        <v>433.08500000000004</v>
       </c>
       <c r="K44">
         <f>J42*G42</f>
-        <v>1269.2935999999995</v>
+        <v>433.08500000000004</v>
       </c>
       <c r="O44" s="3"/>
       <c r="Q44" s="3"/>
@@ -2471,10 +2471,10 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="G48" s="3">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="H48" s="3">
         <v>10000</v>
@@ -2488,39 +2488,39 @@
       </c>
       <c r="K48">
         <f>J48*F48-D48</f>
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="L48">
         <f>J48*G48-E48</f>
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="M48" s="3">
         <f t="shared" ref="M48:M52" si="36">ROUNDDOWN(K48/B48,0)</f>
-        <v>200</v>
+        <v>266</v>
       </c>
       <c r="N48" s="3">
         <f t="shared" ref="N48:N52" si="37">ROUNDDOWN(L48/C48,0)</f>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="O48" s="3">
         <f>M48</f>
-        <v>200</v>
+        <v>266</v>
       </c>
       <c r="P48" s="3">
         <f>N48</f>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="Q48" s="3">
         <f>O48*B48+P48*C48</f>
-        <v>10000</v>
+        <v>9980</v>
       </c>
       <c r="R48" s="3">
         <f>Q48-J48</f>
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="S48">
         <f>M48*B48+N48*C48</f>
-        <v>10000</v>
+        <v>9980</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.3">
@@ -2535,63 +2535,63 @@
       </c>
       <c r="D49">
         <f>O48*B49</f>
-        <v>5640</v>
+        <v>7501.2</v>
       </c>
       <c r="E49">
         <f>P48*C49</f>
-        <v>4160</v>
+        <v>2080</v>
       </c>
       <c r="F49">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="G49" s="3">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="H49" s="3">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="I49">
         <v>0</v>
       </c>
       <c r="J49" s="3">
         <f>D49+E49+H49-I49</f>
-        <v>9800</v>
+        <v>10581.2</v>
       </c>
       <c r="K49">
         <f>J49*F49-D49</f>
-        <v>240</v>
+        <v>963.76000000000113</v>
       </c>
       <c r="L49">
         <f>J49*G49-E49</f>
-        <v>-240</v>
+        <v>36.240000000000236</v>
       </c>
       <c r="M49" s="3">
         <f t="shared" si="36"/>
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="N49" s="3">
         <f t="shared" si="37"/>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="O49" s="3">
         <f>O48+M49</f>
-        <v>208</v>
+        <v>300</v>
       </c>
       <c r="P49" s="3">
         <f>P48+N49</f>
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="Q49" s="3">
         <f t="shared" ref="Q49:Q53" si="38">O49*B49+P49*C49</f>
-        <v>9817.5999999999985</v>
+        <v>10540</v>
       </c>
       <c r="R49" s="3">
         <f t="shared" ref="R49:R53" si="39">Q49-J49</f>
-        <v>17.599999999998545</v>
+        <v>-41.200000000000728</v>
       </c>
       <c r="S49">
         <f t="shared" ref="S49:S53" si="40">M49*B49+N49*C49</f>
-        <v>17.599999999999994</v>
+        <v>958.8</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.3">
@@ -2606,17 +2606,17 @@
       </c>
       <c r="D50">
         <f t="shared" ref="D50:D53" si="41">O49*B50</f>
-        <v>5162.5600000000004</v>
+        <v>7446</v>
       </c>
       <c r="E50">
         <f t="shared" ref="E50:E53" si="42">P49*C50</f>
-        <v>3635.84</v>
+        <v>1913.6000000000001</v>
       </c>
       <c r="F50">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="G50" s="3">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="H50" s="3">
         <v>1000</v>
@@ -2625,44 +2625,44 @@
         <v>0</v>
       </c>
       <c r="J50" s="3">
-        <f t="shared" ref="J50:J53" si="43">D50+E50+H50-I50</f>
-        <v>9798.4000000000015</v>
+        <f t="shared" ref="J50:J52" si="43">D50+E50+H50-I50</f>
+        <v>10359.6</v>
       </c>
       <c r="K50">
         <f t="shared" ref="K50:K53" si="44">J50*F50-D50</f>
-        <v>716.48000000000047</v>
+        <v>841.68000000000029</v>
       </c>
       <c r="L50">
         <f t="shared" ref="L50:L53" si="45">J50*G50-E50</f>
-        <v>283.52000000000044</v>
+        <v>158.31999999999994</v>
       </c>
       <c r="M50" s="3">
         <f t="shared" si="36"/>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="N50" s="3">
         <f t="shared" si="37"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O50" s="3">
         <f t="shared" ref="O50:O53" si="46">O49+M50</f>
-        <v>236</v>
+        <v>333</v>
       </c>
       <c r="P50" s="3">
         <f t="shared" ref="P50:P53" si="47">P49+N50</f>
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="Q50" s="3">
         <f t="shared" si="38"/>
-        <v>9732.5600000000013</v>
+        <v>10322.18</v>
       </c>
       <c r="R50" s="3">
         <f t="shared" si="39"/>
-        <v>-65.840000000000146</v>
+        <v>-37.420000000000073</v>
       </c>
       <c r="S50">
         <f t="shared" si="40"/>
-        <v>934.16000000000008</v>
+        <v>962.58</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.3">
@@ -2677,17 +2677,17 @@
       </c>
       <c r="D51">
         <f t="shared" si="41"/>
-        <v>5680.52</v>
+        <v>8015.31</v>
       </c>
       <c r="E51">
         <f t="shared" si="42"/>
-        <v>4185.2700000000004</v>
+        <v>2221.81</v>
       </c>
       <c r="F51">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="G51" s="3">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="H51" s="3">
         <v>1000</v>
@@ -2697,43 +2697,43 @@
       </c>
       <c r="J51" s="3">
         <f t="shared" si="43"/>
-        <v>10865.79</v>
+        <v>11237.12</v>
       </c>
       <c r="K51">
         <f t="shared" si="44"/>
-        <v>838.95399999999972</v>
+        <v>-149.32600000000002</v>
       </c>
       <c r="L51">
         <f t="shared" si="45"/>
-        <v>161.04600000000028</v>
+        <v>1149.326</v>
       </c>
       <c r="M51" s="3">
         <f t="shared" si="36"/>
-        <v>34</v>
+        <v>-6</v>
       </c>
       <c r="N51" s="3">
         <f t="shared" si="37"/>
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="O51" s="3">
         <f t="shared" si="46"/>
-        <v>270</v>
+        <v>327</v>
       </c>
       <c r="P51" s="3">
         <f t="shared" si="47"/>
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="Q51" s="3">
         <f t="shared" si="38"/>
-        <v>10839.18</v>
+        <v>11229.44</v>
       </c>
       <c r="R51" s="3">
         <f t="shared" si="39"/>
-        <v>-26.610000000000582</v>
+        <v>-7.680000000000291</v>
       </c>
       <c r="S51">
         <f t="shared" si="40"/>
-        <v>973.39</v>
+        <v>992.31999999999994</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.3">
@@ -2748,11 +2748,11 @@
       </c>
       <c r="D52">
         <f t="shared" si="41"/>
-        <v>6955.2000000000007</v>
+        <v>8423.52</v>
       </c>
       <c r="E52">
         <f t="shared" si="42"/>
-        <v>4557</v>
+        <v>3526.25</v>
       </c>
       <c r="F52">
         <v>0.6</v>
@@ -2768,43 +2768,43 @@
       </c>
       <c r="J52" s="3">
         <f t="shared" si="43"/>
-        <v>12512.2</v>
+        <v>12949.77</v>
       </c>
       <c r="K52">
         <f t="shared" si="44"/>
-        <v>552.11999999999898</v>
+        <v>-653.65800000000036</v>
       </c>
       <c r="L52">
         <f t="shared" si="45"/>
-        <v>447.88000000000102</v>
+        <v>1653.6580000000004</v>
       </c>
       <c r="M52" s="3">
         <f t="shared" si="36"/>
-        <v>21</v>
+        <v>-25</v>
       </c>
       <c r="N52" s="3">
         <f t="shared" si="37"/>
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="O52" s="3">
         <f t="shared" si="46"/>
-        <v>291</v>
+        <v>302</v>
       </c>
       <c r="P52" s="3">
         <f t="shared" si="47"/>
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="Q52" s="3">
         <f t="shared" si="38"/>
-        <v>12487.16</v>
+        <v>12933.27</v>
       </c>
       <c r="R52" s="3">
         <f t="shared" si="39"/>
-        <v>-25.040000000000873</v>
+        <v>-16.5</v>
       </c>
       <c r="S52">
         <f t="shared" si="40"/>
-        <v>974.96</v>
+        <v>983.5</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.3">
@@ -2819,63 +2819,61 @@
       </c>
       <c r="D53">
         <f t="shared" si="41"/>
-        <v>9143.2200000000012</v>
+        <v>9488.84</v>
       </c>
       <c r="E53">
         <f t="shared" si="42"/>
-        <v>5140.96</v>
+        <v>5308.6</v>
       </c>
       <c r="F53">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="G53" s="3">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H53" s="3">
         <v>0</v>
       </c>
-      <c r="I53">
-        <v>0</v>
-      </c>
+      <c r="I53" s="3"/>
       <c r="J53" s="3">
         <f>D53+E53+H53-I53</f>
-        <v>14284.18</v>
+        <v>14797.44</v>
       </c>
       <c r="K53" s="3">
         <f t="shared" si="44"/>
-        <v>-572.71200000000135</v>
+        <v>-2090.12</v>
       </c>
       <c r="L53" s="3">
         <f t="shared" si="45"/>
-        <v>572.71200000000044</v>
+        <v>2090.12</v>
       </c>
       <c r="M53" s="3">
         <f>ROUNDDOWN(K53/B53,0)</f>
-        <v>-18</v>
+        <v>-66</v>
       </c>
       <c r="N53" s="3">
         <f>ROUNDDOWN(L53/C53,0)</f>
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="O53" s="3">
         <f t="shared" si="46"/>
-        <v>273</v>
+        <v>236</v>
       </c>
       <c r="P53" s="3">
         <f t="shared" si="47"/>
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="Q53" s="3">
         <f t="shared" si="38"/>
-        <v>14277.42</v>
+        <v>14791.280000000002</v>
       </c>
       <c r="R53" s="3">
         <f t="shared" si="39"/>
-        <v>-6.7600000000002183</v>
+        <v>-6.1599999999980355</v>
       </c>
       <c r="S53" s="3">
         <f t="shared" si="40"/>
-        <v>-6.7599999999999909</v>
+        <v>-6.1600000000003092</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.3">
@@ -2895,15 +2893,15 @@
     <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="I55" s="3">
         <f>J53*0.8</f>
-        <v>11427.344000000001</v>
+        <v>11837.952000000001</v>
       </c>
       <c r="J55" s="3">
         <f>J53*F53</f>
-        <v>8570.5079999999998</v>
+        <v>7398.72</v>
       </c>
       <c r="K55">
         <f>J53*G53</f>
-        <v>5713.6720000000005</v>
+        <v>7398.72</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.3">

</xml_diff>